<commit_message>
Started combining runs into 1 workbook each run is a separate sheet. Necessary busywork for later.
</commit_message>
<xml_diff>
--- a/Excel Workbooks/10/10Pi4.xlsx
+++ b/Excel Workbooks/10/10Pi4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\StatsProject\Excel Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\StatsProject\Excel Workbooks\10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87337E1B-14DF-4BB4-948A-09219FCCC50E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A4B0EE-E795-41ED-9561-A25D31EF16C5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,12 +418,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>